<commit_message>
Ashwini committing for the study phs002371 and 1437
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs001437_DiagAnatomicsite-C40-2-Tibia_Sex-Female_Tumorclass-Primary.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs001437_DiagAnatomicsite-C40-2-Tibia_Sex-Female_Tumorclass-Primary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\03-31-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97B24F6-BB6E-460D-8581-FAAC02E04D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B79DF9-8C3D-480E-8C60-0CA601F56386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="21570" windowHeight="12870" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,185 +116,6 @@
   </si>
   <si>
     <t>TC01_CCDI_phs001437_DiagAnatomicsite-C40-2-Tibia_Sex-Female_Tumorclass-Primary_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>with file_data as (
-select file_name, data_category,file_type, file_size,file_access,  file_description,"sample.id" id from df_sequencing_file
-),
-sample_data1 as (Select smp.id, smp1.sample_id||','|| smp.sample_id as samples, prt.participant_id, prt."study.id" as study FROM 
-   df_sample smp
-LEFT JOIN
-	df_pdx pdx ON smp."pdx.id" = pdx.id
-LEFT JOIN
-	df_sample smp1 ON pdx."sample.id" = smp1.id
-LEFT JOIN
-    df_participant prt ON smp1."participant.id" = prt.id),
-sample_data as (Select smp.id, smp1.sample_id||','|| smp.sample_id as samples, prt.participant_id, prt."study.id" as study FROM 
-   df_sample smp
-LEFT JOIN
-	df_cell_line cl ON smp."cell_line.id" = cl.id
-LEFT JOIN
-	df_sample smp1 ON cl."sample.id" = smp1.id
-LEFT JOIN
-    df_participant prt ON smp1."participant.id" = prt.id)
-SELECT DISTINCT
-    fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type",
-    CASE
-        WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-                ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-            END
-        WHEN fd.file_size &gt;= 1024 * 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-                ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-            END
-        WHEN fd.file_size &gt;= 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-                ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-            END
-        ELSE 
-            CASE 
-                WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-                ELSE ROUND(fd.file_size, 2) || ' Bytes'
-            END
-    END AS "File Size",
-    fd.file_access AS "File Access",
-    std.dbgap_accession AS "Study ID",
-    sd.participant_id AS "Participant ID",
-    sd.samples AS "Sample ID"    
-FROM 
-    df_study std
-LEFT JOIN
-	sample_data sd ON std.id = sd.study
-JOIN 
-    file_data fd ON sd.id = fd.id
-WHERE 
-    std.dbgap_accession = 'phs001437'
-union
-SELECT DISTINCT
-    fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type",
-    CASE
-        WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-                ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-            END
-        WHEN fd.file_size &gt;= 1024 * 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-                ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-            END
-        WHEN fd.file_size &gt;= 1024 THEN
-            CASE 
-                WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-                ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-            END
-        ELSE 
-            CASE 
-                WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT)
-                THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-                ELSE ROUND(fd.file_size, 2) || ' Bytes'
-            END
-    END AS "File Size",
-    fd.file_access AS "File Access",
-    std.dbgap_accession AS "Study ID",
-    sd1.participant_id AS "Participant ID",
-    sd1.samples AS "Sample ID"    
-FROM 
-    df_study std
-LEFT JOIN
-	sample_data1 sd1 ON std.id = sd1.study
-LEFT JOIN
-               diagnosis_summary dgn ON prt.id = dgn.participant_id
-JOIN 
-    file_data fd ON sd1.id = fd.id
-WHERE 
-    std.dbgap_accession = 'phs001437' and prt.sex_at_birth = 'Female' and dgn.anatomic_site ='C40.2 : Tibia' and sd1.tumor_classification ='Primary'</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
-    CASE 
-        WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported'
-        ELSE CAST(smp.participant_age_at_collection AS TEXT)
-    END AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    dgn.diagnosis AS "Sample Diagnosis"
-FROM
-    df_sample smp
-LEFT JOIN df_participant prt ON smp."participant.id" = prt.id
-LEFT JOIN df_study std ON prt."study.id" = std.id
-LEFT JOIN df_diagnosis dgn ON dgn."sample.id" = smp.id
-WHERE
-    std.dbgap_accession = 'phs001437' and prt.sex_at_birth = 'Female' and dgn.anatomic_site ='C40.2 : Tibia' and smp1.tumor_classification ='Primary'
-    AND smp.sample_id IS NOT NULL
-UNION
--- PDX-derived samples linked via their `pdx.id`, then finding the original sample from PDX
-SELECT DISTINCT
-    pdx_smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    pdx_smp.anatomic_site AS "Sample Anatomic Site",
-    CASE 
-        WHEN pdx_smp.participant_age_at_collection = -999 THEN 'Not Reported'
-        ELSE CAST(pdx_smp.participant_age_at_collection AS TEXT)
-    END AS "Age at Sample Collection (days)",
-    COALESCE(pdx_smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(pdx_smp.tumor_classification, '') AS "Sample Tumor Classification",
-    dgn.diagnosis AS "Sample Diagnosis"
-FROM
-    df_sample pdx_smp
-LEFT JOIN df_pdx pdx ON pdx_smp."pdx.id" = pdx.id
-LEFT JOIN df_sample smp1 ON pdx."sample.id" = smp1.id
-LEFT JOIN df_participant prt ON smp1."participant.id" = prt.id
-LEFT JOIN df_study std ON prt."study.id" = std.id
-LEFT JOIN df_diagnosis dgn ON dgn."sample.id" = pdx_smp.id
-WHERE
-    std.dbgap_accession = 'phs001437' and prt.sex_at_birth = 'Female' and dgn.anatomic_site ='C40.2 : Tibia' and smp1.tumor_classification ='Primary'
-    AND pdx_smp.sample_id IS NOT NULL
-UNION
-SELECT DISTINCT
-    cl_smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    cl_smp.anatomic_site AS "Sample Anatomic Site",
-    CASE 
-        WHEN cl_smp.participant_age_at_collection = -999 THEN 'Not Reported'
-        ELSE CAST(cl_smp.participant_age_at_collection AS TEXT)
-    END AS "Age at Sample Collection (days)",
-    COALESCE(cl_smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(cl_smp.tumor_classification, '') AS "Sample Tumor Classification",
-    dgn.diagnosis AS "Sample Diagnosis"
-FROM
-    df_sample cl_smp
-LEFT JOIN df_cell_line cl ON cl.id = cl_smp."cell_line.id"
-LEFT JOIN df_sample smp1 ON cl."sample.id" = smp1.id
-LEFT JOIN df_participant prt ON smp1."participant.id" = prt.id
-LEFT JOIN df_study std ON prt."study.id" = std.id
-LEFT JOIN df_diagnosis dgn ON dgn."sample.id" = cl_smp.id
-WHERE
-    std.dbgap_accession = 'phs001437' and prt.sex_at_birth = 'Female' and dgn.anatomic_site ='C40.2 : Tibia' and smp1.tumor_classification ='Primary'
-    AND cl_smp."cell_line.id" IS NOT NULL</t>
   </si>
   <si>
     <t>WITH diagnosis_summary AS (
@@ -348,48 +169,189 @@
 ;</t>
   </si>
   <si>
-    <t>WITH all_samples AS (
-    -- Direct participant samples
-    SELECT smp.id AS sample_id, prt.participant_id, std.dbgap_accession
+    <t>WITH files AS (
+    SELECT COUNT(DISTINCT sequencing_file_id) AS file_count
+    FROM df_sequencing_file
+    WHERE sequencing_file_id IS NOT NULL
+),
+samples AS (
+    SELECT COUNT(DISTINCT sample_id) AS sample_count
+    FROM df_sample
+    WHERE tumor_classification = 'Primary'
+),
+participants AS (
+    SELECT COUNT(DISTINCT participant_id) AS participant_count
+    FROM df_participant
+    WHERE sex_at_birth = 'Female'
+),
+diagnosis AS (
+    SELECT COUNT(DISTINCT diagnosis_id) AS diagnosis_count
+    FROM df_diagnosis
+    WHERE tumor_classification = 'Primary'
+      AND anatomic_site = 'C40.2 : Tibia'
+)
+SELECT
+    1 AS Studies,  -- We are looking for only one study ('phs001437')
+    p.participant_count AS Participants,  -- Count from participants CTE
+    s.sample_count AS Samples,  -- Count from samples CTE
+    f.file_count AS Files  -- Count from files CTE
+FROM participants p, samples s, files f;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    smp.sample_id AS "Sample ID",
+    prt.participant_id AS "Participant ID",
+    std.dbgap_accession AS "Study ID",
+    smp.anatomic_site AS "Sample Anatomic Site",
+    CASE 
+        WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported'
+        ELSE CAST(smp.participant_age_at_collection AS TEXT)
+    END AS "Age at Sample Collection (days)",
+    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
+    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
+    dgn.diagnosis AS "Sample Diagnosis"
+FROM
+    df_sample smp
+LEFT JOIN df_participant prt ON smp."participant.id" = prt.id
+LEFT JOIN df_study std ON prt."study.id" = std.id
+LEFT JOIN df_diagnosis dgn ON dgn."sample.id" = smp.id
+WHERE
+    std.dbgap_accession = 'phs001437' 
+    AND prt.sex_at_birth = 'Female' 
+    AND dgn.anatomic_site = 'C40.2 : Tibia' 
+    AND smp.tumor_classification = 'Primary'
+    AND smp.sample_id IS NOT NULL
+UNION
+-- PDX-derived samples linked via their `pdx.id`, then finding the original sample from PDX
+SELECT DISTINCT
+    pdx_smp.sample_id AS "Sample ID",
+    prt.participant_id AS "Participant ID",
+    std.dbgap_accession AS "Study ID",
+    pdx_smp.anatomic_site AS "Sample Anatomic Site",
+    CASE 
+        WHEN pdx_smp.participant_age_at_collection = -999 THEN 'Not Reported'
+        ELSE CAST(pdx_smp.participant_age_at_collection AS TEXT)
+    END AS "Age at Sample Collection (days)",
+    COALESCE(pdx_smp.sample_tumor_status, '') AS "Sample Tumor Status",
+    COALESCE(pdx_smp.tumor_classification, '') AS "Sample Tumor Classification",
+    dgn.diagnosis AS "Sample Diagnosis"
+FROM
+    df_sample pdx_smp
+LEFT JOIN df_pdx pdx ON pdx_smp."pdx.id" = pdx.id
+LEFT JOIN df_sample smp1 ON pdx."sample.id" = smp1.id  -- Linking to the original sample
+LEFT JOIN df_participant prt ON smp1."participant.id" = prt.id
+LEFT JOIN df_study std ON prt."study.id" = std.id
+LEFT JOIN df_diagnosis dgn ON dgn."sample.id" = pdx_smp.id
+WHERE
+    std.dbgap_accession = 'phs001437' 
+    AND prt.sex_at_birth = 'Female' 
+    AND dgn.anatomic_site = 'C40.2 : Tibia' 
+    AND smp1.tumor_classification = 'Primary'  -- Fixed the reference here
+    AND pdx_smp.sample_id IS NOT NULL
+UNION
+-- Cell-line derived samples
+SELECT DISTINCT
+    cl_smp.sample_id AS "Sample ID",
+    prt.participant_id AS "Participant ID",
+    std.dbgap_accession AS "Study ID",
+    cl_smp.anatomic_site AS "Sample Anatomic Site",
+    CASE 
+        WHEN cl_smp.participant_age_at_collection = -999 THEN 'Not Reported'
+        ELSE CAST(cl_smp.participant_age_at_collection AS TEXT)
+    END AS "Age at Sample Collection (days)",
+    COALESCE(cl_smp.sample_tumor_status, '') AS "Sample Tumor Status",
+    COALESCE(cl_smp.tumor_classification, '') AS "Sample Tumor Classification",
+    dgn.diagnosis AS "Sample Diagnosis"
+FROM
+    df_sample cl_smp
+LEFT JOIN df_cell_line cl ON cl.id = cl_smp."cell_line.id"
+LEFT JOIN df_sample smp1 ON cl."sample.id" = smp1.id  -- Linking to the original sample
+LEFT JOIN df_participant prt ON smp1."participant.id" = prt.id
+LEFT JOIN df_study std ON prt."study.id" = std.id
+LEFT JOIN df_diagnosis dgn ON dgn."sample.id" = cl_smp.id
+WHERE
+    std.dbgap_accession = 'phs001437' 
+    AND prt.sex_at_birth = 'Female' 
+    AND dgn.anatomic_site = 'C40.2 : Tibia' 
+    AND smp1.tumor_classification = 'Primary'  -- Fixed the reference here
+    AND cl_smp."cell_line.id" IS NOT NULL;</t>
+  </si>
+  <si>
+    <t>WITH file_data AS (
+    SELECT 
+        file_name, 
+        data_category,
+        file_type, 
+        file_size, 
+        file_access,  
+        file_description,
+        "sample.id" AS id
+    FROM df_sequencing_file
+),
+sample_data1 AS (
+    SELECT 
+        smp.id, 
+        smp1.sample_id || ',' || smp.sample_id AS samples, 
+        prt.participant_id, 
+        prt."study.id" AS study,
+        smp.tumor_classification,  
+        prt.sex_at_birth,
+        dgn.anatomic_site
     FROM df_sample smp
-    LEFT JOIN df_participant prt ON smp."participant.id" = prt.id
-    LEFT JOIN df_study std ON prt."study.id" = std.id
-    WHERE smp.sample_id IS NOT NULL
-    UNION
-    -- PDX-derived samples
-    SELECT pdx_smp.id AS sample_id, prt.participant_id, std.dbgap_accession
-    FROM df_sample pdx_smp
-    LEFT JOIN df_pdx pdx ON pdx_smp."pdx.id" = pdx.id
+    LEFT JOIN df_pdx pdx ON smp."pdx.id" = pdx.id
     LEFT JOIN df_sample smp1 ON pdx."sample.id" = smp1.id
     LEFT JOIN df_participant prt ON smp1."participant.id" = prt.id
-    LEFT JOIN df_study std ON prt."study.id" = std.id
-    WHERE pdx_smp.sample_id IS NOT NULL
-    UNION
-    -- Cell line–derived samples using correct cell_line.id
-    SELECT cl_smp.id AS sample_id, prt.participant_id, std.dbgap_accession
-    FROM df_cell_line cl
-    LEFT JOIN df_sample cl_smp ON cl_smp."cell_line.id" = cl.id
-    LEFT JOIN df_sample orig_smp ON cl."sample.id" = orig_smp.id
-    LEFT JOIN df_participant prt ON orig_smp."participant.id" = prt.id
-    LEFT JOIN df_study std ON prt."study.id" = std.id
-    WHERE cl_smp.sample_id IS NOT NULL
+    LEFT JOIN df_diagnosis dgn ON smp.id = dgn.sample_id  -- Change to correct column name here
+),
+sample_data AS (
+    SELECT 
+        smp.id, 
+        smp1.sample_id || ',' || smp.sample_id AS samples, 
+        prt.participant_id, 
+        prt."study.id" AS study
+    FROM df_sample smp
+    LEFT JOIN df_cell_line cl ON smp."cell_line.id" = cl.id
+    LEFT JOIN df_sample smp1 ON cl."sample.id" = smp1.id
+    LEFT JOIN df_participant prt ON smp1."participant.id" = prt.id
 )
-SELECT
-    COUNT(DISTINCT s.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT s.participant_id) AS "Participants",
-    COUNT(DISTINCT s.sample_id) AS "Samples",
-    COUNT(DISTINCT seq.id) AS "Files"
-FROM 
-    all_samples s
-LEFT JOIN df_sequencing_file seq ON s.sample_id = seq."sample.id"
-LEFT JOIN df_participant prt ON s.participant_id = prt.id
-LEFT JOIN df_diagnosis dgn ON prt.id = dgn."participant.id"
-LEFT JOIN df_sample smp1 ON s.sample_id = smp1.id
-WHERE 
-    s.dbgap_accession = 'phs001437'  
-    AND prt.sex_at_birth = 'Female' 
-    AND dgn.anatomic_site = 'C40.2 : Tibia' 
-    AND smp1.tumor_classification = 'Primary';</t>
+SELECT DISTINCT
+    fd.file_name AS "File Name",
+    fd.data_category AS "Data Category",
+    COALESCE(fd.file_description, '') AS "File Description",
+    fd.file_type AS "File Type",
+    CASE
+        WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN
+            CASE 
+                WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
+                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+                ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+            END
+        WHEN fd.file_size &gt;= 1024 * 1024 THEN
+            CASE 
+                WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
+                THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+                ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
+            END
+        WHEN fd.file_size &gt;= 1024 THEN
+            CASE 
+                WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
+                THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+                ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
+            END
+        ELSE '0 KB'  -- Handle cases where file_size is zero or NULL
+    END AS "File Size",
+    sd.samples AS "Sample IDs",
+    sd.participant_id AS "Participant ID",
+    sd.study AS "Study ID",
+    sd1.tumor_classification AS "Tumor Classification",
+    sd1.sex_at_birth AS "Sex at Birth",
+    sd1.anatomic_site AS "Anatomic Site"
+FROM file_data fd
+LEFT JOIN sample_data sd ON fd.id = sd.id
+LEFT JOIN sample_data1 sd1 ON fd.id = sd1.id
+WHERE sd1.sex_at_birth = 'Female'
+  AND sd1.anatomic_site = 'C40.2 : Tibia'
+  AND sd1.tumor_classification = 'Primary';</t>
   </si>
 </sst>
 </file>
@@ -791,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,10 +787,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -851,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -860,7 +822,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -869,6 +831,7 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>